<commit_message>
Forgot to add URL for source
</commit_message>
<xml_diff>
--- a/ConditionalFormattingInPivotTables.xlsx
+++ b/ConditionalFormattingInPivotTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{8DB9FFBA-3C15-4834-AA73-4DFD09F9E485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DB50E9-DDD4-4091-9027-2BB5D861A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,8 +22,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="34">
   <si>
     <t>FROM:</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Total Sum of Value</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zz6F7AcbMzg</t>
   </si>
 </sst>
 </file>
@@ -348,7 +351,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -358,7 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
@@ -970,7 +972,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04DD6752-C11F-4635-B98D-A753E24A8AAF}" name="PivotTable6" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04DD6752-C11F-4635-B98D-A753E24A8AAF}" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="H77:P85" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1122,7 +1124,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2BBA7FD-612F-45CE-B3A1-66FC51FAF0B8}" name="PivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2BBA7FD-612F-45CE-B3A1-66FC51FAF0B8}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="H66:L73" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1214,7 +1216,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7D1C0E90-BD8D-4C5C-BA86-C0F3267DC93F}" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7D1C0E90-BD8D-4C5C-BA86-C0F3267DC93F}" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="H55:L62" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1306,7 +1308,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF39163-511A-4282-9108-6F8C484CE7F1}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FF39163-511A-4282-9108-6F8C484CE7F1}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="H31:K52" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1438,7 +1440,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EAB3F470-20A2-4EC7-A0DB-9400EC891590}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EAB3F470-20A2-4EC7-A0DB-9400EC891590}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="H7:J28" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1561,7 +1563,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1867,8 +1869,8 @@
   </sheetPr>
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P70" sqref="P70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1895,12 +1897,15 @@
         <v>21</v>
       </c>
       <c r="C2" s="2"/>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>45266</v>
       </c>
       <c r="C3" s="2"/>
@@ -1938,7 +1943,6 @@
       <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1953,7 +1957,7 @@
       <c r="I9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9">
         <v>17</v>
       </c>
     </row>
@@ -1970,7 +1974,7 @@
       <c r="I10" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10">
         <v>27</v>
       </c>
     </row>
@@ -1987,7 +1991,7 @@
       <c r="I11" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11">
         <v>37</v>
       </c>
     </row>
@@ -2004,7 +2008,6 @@
       <c r="H12" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2019,7 +2022,7 @@
       <c r="I13" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13">
         <v>29</v>
       </c>
     </row>
@@ -2036,7 +2039,7 @@
       <c r="I14" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14">
         <v>9</v>
       </c>
     </row>
@@ -2053,7 +2056,7 @@
       <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15">
         <v>49</v>
       </c>
     </row>
@@ -2070,7 +2073,6 @@
       <c r="H16" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2085,7 +2087,7 @@
       <c r="I17" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17">
         <v>41</v>
       </c>
     </row>
@@ -2102,7 +2104,7 @@
       <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18">
         <v>21</v>
       </c>
     </row>
@@ -2119,7 +2121,7 @@
       <c r="I19" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19">
         <v>31</v>
       </c>
     </row>
@@ -2136,7 +2138,6 @@
       <c r="H20" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -2151,7 +2152,7 @@
       <c r="I21" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21">
         <v>53</v>
       </c>
     </row>
@@ -2168,7 +2169,7 @@
       <c r="I22" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22">
         <v>33</v>
       </c>
     </row>
@@ -2185,7 +2186,7 @@
       <c r="I23" t="s">
         <v>27</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23">
         <v>13</v>
       </c>
     </row>
@@ -2202,7 +2203,6 @@
       <c r="H24" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -2217,7 +2217,7 @@
       <c r="I25" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25">
         <v>35</v>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       <c r="I26" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26">
         <v>45</v>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
       <c r="I27" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27">
         <v>25</v>
       </c>
     </row>
@@ -2268,7 +2268,7 @@
       <c r="H28" t="s">
         <v>13</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28">
         <v>465</v>
       </c>
     </row>
@@ -2330,8 +2330,6 @@
       <c r="H32" t="s">
         <v>8</v>
       </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -2346,10 +2344,10 @@
       <c r="I33" t="s">
         <v>28</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33">
         <v>17</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33">
         <v>17</v>
       </c>
     </row>
@@ -2366,10 +2364,10 @@
       <c r="I34" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34">
         <v>27</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34">
         <v>27</v>
       </c>
     </row>
@@ -2386,10 +2384,10 @@
       <c r="I35" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35">
         <v>37</v>
       </c>
-      <c r="K35" s="9">
+      <c r="K35">
         <v>37</v>
       </c>
     </row>
@@ -2406,8 +2404,6 @@
       <c r="H36" t="s">
         <v>9</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2422,10 +2418,10 @@
       <c r="I37" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37">
         <v>29</v>
       </c>
-      <c r="K37" s="9">
+      <c r="K37">
         <v>29</v>
       </c>
     </row>
@@ -2433,10 +2429,10 @@
       <c r="I38" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38">
         <v>9</v>
       </c>
-      <c r="K38" s="9">
+      <c r="K38">
         <v>9</v>
       </c>
     </row>
@@ -2444,10 +2440,10 @@
       <c r="I39" t="s">
         <v>27</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39">
         <v>49</v>
       </c>
-      <c r="K39" s="9">
+      <c r="K39">
         <v>49</v>
       </c>
     </row>
@@ -2455,17 +2451,15 @@
       <c r="H40" t="s">
         <v>10</v>
       </c>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41">
         <v>41</v>
       </c>
-      <c r="K41" s="9">
+      <c r="K41">
         <v>41</v>
       </c>
     </row>
@@ -2473,10 +2467,10 @@
       <c r="I42" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42">
         <v>21</v>
       </c>
-      <c r="K42" s="9">
+      <c r="K42">
         <v>21</v>
       </c>
     </row>
@@ -2484,10 +2478,10 @@
       <c r="I43" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43">
         <v>31</v>
       </c>
-      <c r="K43" s="9">
+      <c r="K43">
         <v>31</v>
       </c>
     </row>
@@ -2495,17 +2489,15 @@
       <c r="H44" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I45" t="s">
         <v>28</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45">
         <v>53</v>
       </c>
-      <c r="K45" s="9">
+      <c r="K45">
         <v>53</v>
       </c>
     </row>
@@ -2513,10 +2505,10 @@
       <c r="I46" t="s">
         <v>26</v>
       </c>
-      <c r="J46" s="9">
+      <c r="J46">
         <v>33</v>
       </c>
-      <c r="K46" s="9">
+      <c r="K46">
         <v>33</v>
       </c>
     </row>
@@ -2524,10 +2516,10 @@
       <c r="I47" t="s">
         <v>27</v>
       </c>
-      <c r="J47" s="9">
+      <c r="J47">
         <v>13</v>
       </c>
-      <c r="K47" s="9">
+      <c r="K47">
         <v>13</v>
       </c>
     </row>
@@ -2535,17 +2527,15 @@
       <c r="H48" t="s">
         <v>24</v>
       </c>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
     </row>
     <row r="49" spans="8:12" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
         <v>28</v>
       </c>
-      <c r="J49" s="9">
+      <c r="J49">
         <v>35</v>
       </c>
-      <c r="K49" s="9">
+      <c r="K49">
         <v>35</v>
       </c>
     </row>
@@ -2553,10 +2543,10 @@
       <c r="I50" t="s">
         <v>26</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J50">
         <v>45</v>
       </c>
-      <c r="K50" s="9">
+      <c r="K50">
         <v>45</v>
       </c>
     </row>
@@ -2564,10 +2554,10 @@
       <c r="I51" t="s">
         <v>27</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51">
         <v>25</v>
       </c>
-      <c r="K51" s="9">
+      <c r="K51">
         <v>25</v>
       </c>
     </row>
@@ -2575,10 +2565,10 @@
       <c r="H52" t="s">
         <v>13</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52">
         <v>465</v>
       </c>
-      <c r="K52" s="9">
+      <c r="K52">
         <v>465</v>
       </c>
     </row>
@@ -2611,16 +2601,16 @@
       <c r="H57" t="s">
         <v>8</v>
       </c>
-      <c r="I57" s="9">
+      <c r="I57">
         <v>17</v>
       </c>
-      <c r="J57" s="9">
+      <c r="J57">
         <v>27</v>
       </c>
-      <c r="K57" s="9">
+      <c r="K57">
         <v>37</v>
       </c>
-      <c r="L57" s="9">
+      <c r="L57">
         <v>81</v>
       </c>
     </row>
@@ -2628,16 +2618,16 @@
       <c r="H58" t="s">
         <v>9</v>
       </c>
-      <c r="I58" s="9">
+      <c r="I58">
         <v>29</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58">
         <v>9</v>
       </c>
-      <c r="K58" s="9">
+      <c r="K58">
         <v>49</v>
       </c>
-      <c r="L58" s="9">
+      <c r="L58">
         <v>87</v>
       </c>
     </row>
@@ -2645,16 +2635,16 @@
       <c r="H59" t="s">
         <v>10</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59">
         <v>41</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59">
         <v>21</v>
       </c>
-      <c r="K59" s="9">
+      <c r="K59">
         <v>31</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59">
         <v>93</v>
       </c>
     </row>
@@ -2662,16 +2652,16 @@
       <c r="H60" t="s">
         <v>23</v>
       </c>
-      <c r="I60" s="9">
+      <c r="I60">
         <v>53</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60">
         <v>33</v>
       </c>
-      <c r="K60" s="9">
+      <c r="K60">
         <v>13</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60">
         <v>99</v>
       </c>
     </row>
@@ -2679,16 +2669,16 @@
       <c r="H61" t="s">
         <v>24</v>
       </c>
-      <c r="I61" s="9">
+      <c r="I61">
         <v>35</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61">
         <v>45</v>
       </c>
-      <c r="K61" s="9">
+      <c r="K61">
         <v>25</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61">
         <v>105</v>
       </c>
     </row>
@@ -2696,16 +2686,16 @@
       <c r="H62" t="s">
         <v>13</v>
       </c>
-      <c r="I62" s="9">
+      <c r="I62">
         <v>175</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62">
         <v>135</v>
       </c>
-      <c r="K62" s="9">
+      <c r="K62">
         <v>155</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62">
         <v>465</v>
       </c>
     </row>
@@ -2738,16 +2728,16 @@
       <c r="H68" t="s">
         <v>8</v>
       </c>
-      <c r="I68" s="9">
+      <c r="I68">
         <v>17</v>
       </c>
-      <c r="J68" s="9">
+      <c r="J68">
         <v>27</v>
       </c>
-      <c r="K68" s="9">
+      <c r="K68">
         <v>37</v>
       </c>
-      <c r="L68" s="9">
+      <c r="L68">
         <v>81</v>
       </c>
     </row>
@@ -2755,16 +2745,16 @@
       <c r="H69" t="s">
         <v>9</v>
       </c>
-      <c r="I69" s="9">
+      <c r="I69">
         <v>29</v>
       </c>
-      <c r="J69" s="9">
+      <c r="J69">
         <v>9</v>
       </c>
-      <c r="K69" s="9">
+      <c r="K69">
         <v>49</v>
       </c>
-      <c r="L69" s="9">
+      <c r="L69">
         <v>87</v>
       </c>
     </row>
@@ -2772,16 +2762,16 @@
       <c r="H70" t="s">
         <v>10</v>
       </c>
-      <c r="I70" s="9">
+      <c r="I70">
         <v>41</v>
       </c>
-      <c r="J70" s="9">
+      <c r="J70">
         <v>21</v>
       </c>
-      <c r="K70" s="9">
+      <c r="K70">
         <v>31</v>
       </c>
-      <c r="L70" s="9">
+      <c r="L70">
         <v>93</v>
       </c>
     </row>
@@ -2789,16 +2779,16 @@
       <c r="H71" t="s">
         <v>23</v>
       </c>
-      <c r="I71" s="9">
+      <c r="I71">
         <v>53</v>
       </c>
-      <c r="J71" s="9">
+      <c r="J71">
         <v>33</v>
       </c>
-      <c r="K71" s="9">
+      <c r="K71">
         <v>13</v>
       </c>
-      <c r="L71" s="9">
+      <c r="L71">
         <v>99</v>
       </c>
     </row>
@@ -2806,16 +2796,16 @@
       <c r="H72" t="s">
         <v>24</v>
       </c>
-      <c r="I72" s="9">
+      <c r="I72">
         <v>35</v>
       </c>
-      <c r="J72" s="9">
+      <c r="J72">
         <v>45</v>
       </c>
-      <c r="K72" s="9">
+      <c r="K72">
         <v>25</v>
       </c>
-      <c r="L72" s="9">
+      <c r="L72">
         <v>105</v>
       </c>
     </row>
@@ -2823,16 +2813,16 @@
       <c r="H73" t="s">
         <v>13</v>
       </c>
-      <c r="I73" s="9">
+      <c r="I73">
         <v>175</v>
       </c>
-      <c r="J73" s="9">
+      <c r="J73">
         <v>135</v>
       </c>
-      <c r="K73" s="9">
+      <c r="K73">
         <v>155</v>
       </c>
-      <c r="L73" s="9">
+      <c r="L73">
         <v>465</v>
       </c>
     </row>
@@ -2888,28 +2878,28 @@
       <c r="H80" t="s">
         <v>8</v>
       </c>
-      <c r="I80" s="9">
+      <c r="I80">
         <v>17</v>
       </c>
-      <c r="J80" s="9">
+      <c r="J80">
         <v>17</v>
       </c>
-      <c r="K80" s="9">
+      <c r="K80">
         <v>27</v>
       </c>
-      <c r="L80" s="9">
+      <c r="L80">
         <v>27</v>
       </c>
-      <c r="M80" s="9">
+      <c r="M80">
         <v>37</v>
       </c>
-      <c r="N80" s="9">
+      <c r="N80">
         <v>37</v>
       </c>
-      <c r="O80" s="9">
+      <c r="O80">
         <v>81</v>
       </c>
-      <c r="P80" s="9">
+      <c r="P80">
         <v>81</v>
       </c>
     </row>
@@ -2917,28 +2907,28 @@
       <c r="H81" t="s">
         <v>9</v>
       </c>
-      <c r="I81" s="9">
+      <c r="I81">
         <v>29</v>
       </c>
-      <c r="J81" s="9">
+      <c r="J81">
         <v>29</v>
       </c>
-      <c r="K81" s="9">
+      <c r="K81">
         <v>9</v>
       </c>
-      <c r="L81" s="9">
+      <c r="L81">
         <v>9</v>
       </c>
-      <c r="M81" s="9">
+      <c r="M81">
         <v>49</v>
       </c>
-      <c r="N81" s="9">
+      <c r="N81">
         <v>49</v>
       </c>
-      <c r="O81" s="9">
+      <c r="O81">
         <v>87</v>
       </c>
-      <c r="P81" s="9">
+      <c r="P81">
         <v>87</v>
       </c>
     </row>
@@ -2946,28 +2936,28 @@
       <c r="H82" t="s">
         <v>10</v>
       </c>
-      <c r="I82" s="9">
+      <c r="I82">
         <v>41</v>
       </c>
-      <c r="J82" s="9">
+      <c r="J82">
         <v>41</v>
       </c>
-      <c r="K82" s="9">
+      <c r="K82">
         <v>21</v>
       </c>
-      <c r="L82" s="9">
+      <c r="L82">
         <v>21</v>
       </c>
-      <c r="M82" s="9">
+      <c r="M82">
         <v>31</v>
       </c>
-      <c r="N82" s="9">
+      <c r="N82">
         <v>31</v>
       </c>
-      <c r="O82" s="9">
+      <c r="O82">
         <v>93</v>
       </c>
-      <c r="P82" s="9">
+      <c r="P82">
         <v>93</v>
       </c>
     </row>
@@ -2975,28 +2965,28 @@
       <c r="H83" t="s">
         <v>23</v>
       </c>
-      <c r="I83" s="9">
+      <c r="I83">
         <v>53</v>
       </c>
-      <c r="J83" s="9">
+      <c r="J83">
         <v>53</v>
       </c>
-      <c r="K83" s="9">
+      <c r="K83">
         <v>33</v>
       </c>
-      <c r="L83" s="9">
+      <c r="L83">
         <v>33</v>
       </c>
-      <c r="M83" s="9">
+      <c r="M83">
         <v>13</v>
       </c>
-      <c r="N83" s="9">
+      <c r="N83">
         <v>13</v>
       </c>
-      <c r="O83" s="9">
+      <c r="O83">
         <v>99</v>
       </c>
-      <c r="P83" s="9">
+      <c r="P83">
         <v>99</v>
       </c>
     </row>
@@ -3004,28 +2994,28 @@
       <c r="H84" t="s">
         <v>24</v>
       </c>
-      <c r="I84" s="9">
+      <c r="I84">
         <v>35</v>
       </c>
-      <c r="J84" s="9">
+      <c r="J84">
         <v>35</v>
       </c>
-      <c r="K84" s="9">
+      <c r="K84">
         <v>45</v>
       </c>
-      <c r="L84" s="9">
+      <c r="L84">
         <v>45</v>
       </c>
-      <c r="M84" s="9">
+      <c r="M84">
         <v>25</v>
       </c>
-      <c r="N84" s="9">
+      <c r="N84">
         <v>25</v>
       </c>
-      <c r="O84" s="9">
+      <c r="O84">
         <v>105</v>
       </c>
-      <c r="P84" s="9">
+      <c r="P84">
         <v>105</v>
       </c>
     </row>
@@ -3033,28 +3023,28 @@
       <c r="H85" t="s">
         <v>13</v>
       </c>
-      <c r="I85" s="9">
+      <c r="I85">
         <v>175</v>
       </c>
-      <c r="J85" s="9">
+      <c r="J85">
         <v>175</v>
       </c>
-      <c r="K85" s="9">
+      <c r="K85">
         <v>135</v>
       </c>
-      <c r="L85" s="9">
+      <c r="L85">
         <v>135</v>
       </c>
-      <c r="M85" s="9">
+      <c r="M85">
         <v>155</v>
       </c>
-      <c r="N85" s="9">
+      <c r="N85">
         <v>155</v>
       </c>
-      <c r="O85" s="9">
+      <c r="O85">
         <v>465</v>
       </c>
-      <c r="P85" s="9">
+      <c r="P85">
         <v>465</v>
       </c>
     </row>
@@ -3204,7 +3194,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>06-Dec-2023</v>
+        <v>13-Dec-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3340,19 +3330,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -3360,11 +3346,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -3372,19 +3357,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -3392,11 +3373,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -3404,19 +3384,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -3424,11 +3400,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -3436,13 +3411,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -3515,7 +3490,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>06-Dec-2023</v>
+        <v>13-Dec-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>